<commit_message>
fail template footer restoration need to fix
</commit_message>
<xml_diff>
--- a/result_footer_test.xlsx
+++ b/result_footer_test.xlsx
@@ -219,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -258,6 +258,14 @@
       <bottom style="thin">
         <color rgb="00000000"/>
       </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
     </border>
     <border>
       <left style="thin">
@@ -329,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -490,6 +498,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -552,11 +563,11 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -564,6 +575,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1620,7 +1646,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O46"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2450,210 +2476,223 @@
       </c>
     </row>
     <row r="37" ht="35" customHeight="1">
-      <c r="A37" s="54" t="n"/>
+      <c r="A37" s="60" t="n"/>
       <c r="B37" s="54" t="inlineStr">
         <is>
+          <t>HS.CODE: 4107.12.00</t>
+        </is>
+      </c>
+      <c r="C37" s="54" t="n"/>
+      <c r="D37" s="55" t="n"/>
+      <c r="E37" s="56" t="n"/>
+      <c r="F37" s="56" t="n"/>
+      <c r="G37" s="56" t="n"/>
+    </row>
+    <row r="38" ht="35" customHeight="1">
+      <c r="A38" s="54" t="n"/>
+      <c r="B38" s="54" t="inlineStr">
+        <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="C37" s="54" t="inlineStr">
+      <c r="C38" s="54" t="inlineStr">
         <is>
           <t>31 PALLETS</t>
         </is>
       </c>
-      <c r="D37" s="55" t="n"/>
-      <c r="E37" s="56">
+      <c r="D38" s="55" t="n"/>
+      <c r="E38" s="56">
         <f>SUM(E22:E36)</f>
         <v/>
       </c>
-      <c r="F37" s="56" t="n"/>
-      <c r="G37" s="56">
+      <c r="F38" s="56" t="n"/>
+      <c r="G38" s="56">
         <f>SUM(G22:G36)</f>
         <v/>
       </c>
     </row>
-    <row r="38" ht="61.5" customHeight="1">
-      <c r="A38" s="60" t="inlineStr">
+    <row r="39" ht="61.5" customHeight="1">
+      <c r="A39" s="61" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B38" s="61" t="inlineStr">
+      <c r="B39" s="62" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="D38" s="61" t="n"/>
-      <c r="E38" s="61" t="n"/>
-      <c r="F38" s="32" t="n"/>
-      <c r="G38" s="26" t="n"/>
-      <c r="H38" s="2" t="n"/>
-      <c r="I38" s="2" t="n"/>
-      <c r="J38" s="2" t="n"/>
-      <c r="K38" s="2" t="n"/>
-      <c r="L38" s="62" t="n"/>
-      <c r="M38" s="63" t="n"/>
-      <c r="N38" s="64" t="n"/>
-      <c r="O38" s="64" t="n"/>
-    </row>
-    <row r="39" ht="42" customHeight="1">
-      <c r="A39" s="65" t="inlineStr">
-        <is>
-          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
-                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
-      <c r="D39" s="65" t="n"/>
-      <c r="E39" s="65" t="n"/>
-      <c r="F39" s="65" t="n"/>
+      <c r="D39" s="62" t="n"/>
+      <c r="E39" s="62" t="n"/>
+      <c r="F39" s="32" t="n"/>
       <c r="G39" s="26" t="n"/>
       <c r="H39" s="2" t="n"/>
       <c r="I39" s="2" t="n"/>
       <c r="J39" s="2" t="n"/>
       <c r="K39" s="2" t="n"/>
-      <c r="L39" s="62" t="n"/>
-      <c r="M39" s="63" t="n"/>
-      <c r="N39" s="64" t="n"/>
-      <c r="O39" s="64" t="n"/>
-    </row>
-    <row r="40" ht="24.75" customHeight="1">
+      <c r="L39" s="63" t="n"/>
+      <c r="M39" s="64" t="n"/>
+      <c r="N39" s="65" t="n"/>
+      <c r="O39" s="65" t="n"/>
+    </row>
+    <row r="40" ht="42" customHeight="1">
       <c r="A40" s="66" t="inlineStr">
         <is>
-          <t>A/C NO:100001100764430</t>
-        </is>
-      </c>
+          <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
+                                                  /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+      <c r="D40" s="66" t="n"/>
+      <c r="E40" s="66" t="n"/>
+      <c r="F40" s="66" t="n"/>
+      <c r="G40" s="26" t="n"/>
       <c r="H40" s="2" t="n"/>
       <c r="I40" s="2" t="n"/>
       <c r="J40" s="2" t="n"/>
       <c r="K40" s="2" t="n"/>
-      <c r="L40" s="62" t="n"/>
-      <c r="M40" s="63" t="n"/>
-      <c r="N40" s="64" t="n"/>
-      <c r="O40" s="64" t="n"/>
-    </row>
-    <row r="41" ht="27" customHeight="1">
-      <c r="A41" s="66" t="inlineStr">
-        <is>
-          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+      <c r="L40" s="63" t="n"/>
+      <c r="M40" s="64" t="n"/>
+      <c r="N40" s="65" t="n"/>
+      <c r="O40" s="65" t="n"/>
+    </row>
+    <row r="41" ht="24.75" customHeight="1">
+      <c r="A41" s="67" t="inlineStr">
+        <is>
+          <t>A/C NO:100001100764430</t>
         </is>
       </c>
       <c r="H41" s="2" t="n"/>
       <c r="I41" s="2" t="n"/>
       <c r="J41" s="2" t="n"/>
       <c r="K41" s="2" t="n"/>
-      <c r="L41" s="62" t="n"/>
-      <c r="M41" s="63" t="n"/>
-      <c r="N41" s="64" t="n"/>
-      <c r="O41" s="64" t="n"/>
-    </row>
-    <row r="42" ht="61.5" customHeight="1">
-      <c r="A42" s="2" t="n"/>
-      <c r="B42" s="2" t="n"/>
-      <c r="C42" s="2" t="n"/>
-      <c r="D42" s="2" t="n"/>
-      <c r="E42" s="67" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
-        </is>
-      </c>
-      <c r="F42" s="67" t="n"/>
-      <c r="G42" s="67" t="n"/>
-      <c r="H42" s="67" t="n"/>
+      <c r="L41" s="63" t="n"/>
+      <c r="M41" s="64" t="n"/>
+      <c r="N41" s="65" t="n"/>
+      <c r="O41" s="65" t="n"/>
+    </row>
+    <row r="42" ht="27" customHeight="1">
+      <c r="A42" s="67" t="inlineStr">
+        <is>
+          <t>SWIFT CODE  ：BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="H42" s="2" t="n"/>
       <c r="I42" s="2" t="n"/>
       <c r="J42" s="2" t="n"/>
       <c r="K42" s="2" t="n"/>
-      <c r="L42" s="62" t="n"/>
-      <c r="M42" s="63" t="n"/>
-      <c r="N42" s="64" t="n"/>
-      <c r="O42" s="64" t="n"/>
-    </row>
-    <row r="43" ht="42" customHeight="1">
+      <c r="L42" s="63" t="n"/>
+      <c r="M42" s="64" t="n"/>
+      <c r="N42" s="65" t="n"/>
+      <c r="O42" s="65" t="n"/>
+    </row>
+    <row r="43" ht="61.5" customHeight="1">
       <c r="A43" s="2" t="n"/>
       <c r="B43" s="2" t="n"/>
       <c r="C43" s="2" t="n"/>
-      <c r="D43" s="68" t="n"/>
-      <c r="E43" s="69" t="n"/>
-      <c r="F43" s="70" t="inlineStr">
-        <is>
-          <t>Sign &amp; Stamp</t>
-        </is>
-      </c>
-      <c r="G43" s="71" t="n"/>
-      <c r="H43" s="2" t="n"/>
+      <c r="D43" s="2" t="n"/>
+      <c r="E43" s="68" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
+        </is>
+      </c>
+      <c r="F43" s="68" t="n"/>
+      <c r="G43" s="68" t="n"/>
+      <c r="H43" s="68" t="n"/>
       <c r="I43" s="2" t="n"/>
       <c r="J43" s="2" t="n"/>
       <c r="K43" s="2" t="n"/>
-      <c r="L43" s="62" t="n"/>
-      <c r="M43" s="63" t="n"/>
-      <c r="N43" s="64" t="n"/>
-      <c r="O43" s="64" t="n"/>
-    </row>
-    <row r="44" ht="24.75" customHeight="1">
+      <c r="L43" s="63" t="n"/>
+      <c r="M43" s="64" t="n"/>
+      <c r="N43" s="65" t="n"/>
+      <c r="O43" s="65" t="n"/>
+    </row>
+    <row r="44" ht="42" customHeight="1">
       <c r="A44" s="2" t="n"/>
       <c r="B44" s="2" t="n"/>
       <c r="C44" s="2" t="n"/>
-      <c r="D44" s="68" t="n"/>
-      <c r="E44" s="69" t="n"/>
-      <c r="F44" s="69" t="n"/>
-      <c r="G44" s="71" t="n"/>
+      <c r="D44" s="69" t="n"/>
+      <c r="E44" s="70" t="n"/>
+      <c r="F44" s="71" t="inlineStr">
+        <is>
+          <t>Sign &amp; Stamp</t>
+        </is>
+      </c>
+      <c r="G44" s="72" t="n"/>
       <c r="H44" s="2" t="n"/>
       <c r="I44" s="2" t="n"/>
       <c r="J44" s="2" t="n"/>
       <c r="K44" s="2" t="n"/>
-      <c r="L44" s="62" t="n"/>
-      <c r="M44" s="63" t="n"/>
-      <c r="N44" s="64" t="n"/>
-      <c r="O44" s="64" t="n"/>
-    </row>
-    <row r="45" ht="27" customHeight="1">
+      <c r="L44" s="63" t="n"/>
+      <c r="M44" s="64" t="n"/>
+      <c r="N44" s="65" t="n"/>
+      <c r="O44" s="65" t="n"/>
+    </row>
+    <row r="45" ht="24.75" customHeight="1">
       <c r="A45" s="2" t="n"/>
       <c r="B45" s="2" t="n"/>
       <c r="C45" s="2" t="n"/>
-      <c r="D45" s="68" t="n"/>
-      <c r="E45" s="69" t="n"/>
-      <c r="F45" s="69" t="n"/>
-      <c r="G45" s="71" t="n"/>
+      <c r="D45" s="69" t="n"/>
+      <c r="E45" s="70" t="n"/>
+      <c r="F45" s="70" t="n"/>
+      <c r="G45" s="72" t="n"/>
       <c r="H45" s="2" t="n"/>
       <c r="I45" s="2" t="n"/>
       <c r="J45" s="2" t="n"/>
       <c r="K45" s="2" t="n"/>
-      <c r="L45" s="62" t="n"/>
-      <c r="M45" s="63" t="n"/>
-      <c r="N45" s="64" t="n"/>
-      <c r="O45" s="64" t="n"/>
-    </row>
-    <row r="46" ht="21" customHeight="1">
+      <c r="L45" s="63" t="n"/>
+      <c r="M45" s="64" t="n"/>
+      <c r="N45" s="65" t="n"/>
+      <c r="O45" s="65" t="n"/>
+    </row>
+    <row r="46" ht="27" customHeight="1">
       <c r="A46" s="2" t="n"/>
       <c r="B46" s="2" t="n"/>
       <c r="C46" s="2" t="n"/>
-      <c r="D46" s="68" t="n"/>
-      <c r="E46" s="69" t="n"/>
-      <c r="F46" s="72" t="inlineStr">
-        <is>
-          <t>ZENG XUELI</t>
-        </is>
-      </c>
+      <c r="D46" s="69" t="n"/>
+      <c r="E46" s="70" t="n"/>
+      <c r="F46" s="70" t="n"/>
       <c r="G46" s="72" t="n"/>
       <c r="H46" s="2" t="n"/>
       <c r="I46" s="2" t="n"/>
       <c r="J46" s="2" t="n"/>
       <c r="K46" s="2" t="n"/>
-      <c r="L46" s="62" t="n"/>
-      <c r="M46" s="63" t="n"/>
-      <c r="N46" s="64" t="n"/>
-      <c r="O46" s="64" t="n"/>
+      <c r="L46" s="63" t="n"/>
+      <c r="M46" s="64" t="n"/>
+      <c r="N46" s="65" t="n"/>
+      <c r="O46" s="65" t="n"/>
+    </row>
+    <row r="47" ht="21" customHeight="1">
+      <c r="A47" s="2" t="n"/>
+      <c r="B47" s="2" t="n"/>
+      <c r="C47" s="2" t="n"/>
+      <c r="D47" s="69" t="n"/>
+      <c r="E47" s="70" t="n"/>
+      <c r="F47" s="73" t="inlineStr">
+        <is>
+          <t>ZENG XUELI</t>
+        </is>
+      </c>
+      <c r="G47" s="73" t="n"/>
+      <c r="H47" s="2" t="n"/>
+      <c r="I47" s="2" t="n"/>
+      <c r="J47" s="2" t="n"/>
+      <c r="K47" s="2" t="n"/>
+      <c r="L47" s="63" t="n"/>
+      <c r="M47" s="64" t="n"/>
+      <c r="N47" s="65" t="n"/>
+      <c r="O47" s="65" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A40:G40"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
     <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A40:C40"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A42:G42"/>
     <mergeCell ref="A41:G41"/>
     <mergeCell ref="A5:G5"/>
   </mergeCells>
@@ -2667,7 +2706,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T76"/>
+  <dimension ref="A1:T75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2823,7 +2862,7 @@
     </row>
     <row r="7" ht="18" customHeight="1">
       <c r="A7" s="32" t="n"/>
-      <c r="B7" s="73" t="n"/>
+      <c r="B7" s="74" t="n"/>
       <c r="C7" s="32" t="n"/>
       <c r="D7" s="32" t="n"/>
       <c r="E7" s="26" t="n"/>
@@ -2834,7 +2873,7 @@
           <t>Ref No.:</t>
         </is>
       </c>
-      <c r="I7" s="74" t="inlineStr">
+      <c r="I7" s="75" t="inlineStr">
         <is>
           <t>JFREF</t>
         </is>
@@ -2857,7 +2896,7 @@
           <t>EXPORTER:</t>
         </is>
       </c>
-      <c r="B8" s="75" t="inlineStr">
+      <c r="B8" s="76" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
@@ -2872,7 +2911,7 @@
           <t>INVOICE NO :</t>
         </is>
       </c>
-      <c r="I8" s="76" t="inlineStr">
+      <c r="I8" s="77" t="inlineStr">
         <is>
           <t>JFINV</t>
         </is>
@@ -2891,7 +2930,7 @@
     </row>
     <row r="9" ht="21" customHeight="1">
       <c r="A9" s="32" t="n"/>
-      <c r="B9" s="73" t="inlineStr">
+      <c r="B9" s="74" t="inlineStr">
         <is>
           <t>XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages,</t>
         </is>
@@ -2925,7 +2964,7 @@
     </row>
     <row r="10" ht="22.5" customHeight="1">
       <c r="A10" s="32" t="n"/>
-      <c r="B10" s="73" t="inlineStr">
+      <c r="B10" s="74" t="inlineStr">
         <is>
           <t>Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia</t>
         </is>
@@ -2940,7 +2979,7 @@
           <t>FCA :</t>
         </is>
       </c>
-      <c r="I10" s="77" t="inlineStr">
+      <c r="I10" s="78" t="inlineStr">
         <is>
           <t>BAVET, SVAY RIENG</t>
         </is>
@@ -2959,7 +2998,7 @@
     </row>
     <row r="11" ht="20.25" customHeight="1">
       <c r="A11" s="32" t="n"/>
-      <c r="B11" s="73" t="inlineStr">
+      <c r="B11" s="74" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
@@ -2985,7 +3024,7 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="32" t="n"/>
-      <c r="B12" s="73" t="n"/>
+      <c r="B12" s="74" t="n"/>
       <c r="C12" s="32" t="n"/>
       <c r="D12" s="32" t="n"/>
       <c r="E12" s="26" t="n"/>
@@ -3011,7 +3050,7 @@
           <t>CONSIGNEE :</t>
         </is>
       </c>
-      <c r="B13" s="78" t="inlineStr">
+      <c r="B13" s="79" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
@@ -3019,9 +3058,9 @@
       <c r="C13" s="2" t="n"/>
       <c r="D13" s="2" t="n"/>
       <c r="E13" s="2" t="n"/>
-      <c r="F13" s="79" t="n"/>
-      <c r="G13" s="79" t="n"/>
-      <c r="H13" s="79" t="n"/>
+      <c r="F13" s="80" t="n"/>
+      <c r="G13" s="80" t="n"/>
+      <c r="H13" s="80" t="n"/>
       <c r="I13" s="45" t="n"/>
       <c r="J13" s="2" t="n"/>
       <c r="K13" s="2" t="n"/>
@@ -3037,17 +3076,17 @@
     </row>
     <row r="14" ht="25.5" customHeight="1">
       <c r="A14" s="32" t="n"/>
-      <c r="B14" s="80" t="inlineStr">
+      <c r="B14" s="81" t="inlineStr">
         <is>
           <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
         </is>
       </c>
       <c r="C14" s="47" t="n"/>
       <c r="D14" s="47" t="n"/>
-      <c r="E14" s="81" t="n"/>
-      <c r="F14" s="81" t="n"/>
-      <c r="G14" s="81" t="n"/>
-      <c r="H14" s="81" t="n"/>
+      <c r="E14" s="82" t="n"/>
+      <c r="F14" s="82" t="n"/>
+      <c r="G14" s="82" t="n"/>
+      <c r="H14" s="82" t="n"/>
       <c r="I14" s="2" t="n"/>
       <c r="J14" s="2" t="n"/>
       <c r="K14" s="2" t="n"/>
@@ -3063,7 +3102,7 @@
     </row>
     <row r="15" ht="21" customHeight="1">
       <c r="A15" s="32" t="n"/>
-      <c r="B15" s="82" t="inlineStr">
+      <c r="B15" s="83" t="inlineStr">
         <is>
           <t>BINH PHUOC WARD,DONG NAI PROVINCE, VIETNAM</t>
         </is>
@@ -3171,7 +3210,7 @@
           <t xml:space="preserve">SHIP: </t>
         </is>
       </c>
-      <c r="B19" s="73" t="inlineStr">
+      <c r="B19" s="74" t="inlineStr">
         <is>
           <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO DONG NAI PROVINCE, VIETNAM.</t>
         </is>
@@ -3197,7 +3236,7 @@
     </row>
     <row r="20" ht="27.75" customHeight="1">
       <c r="A20" s="53" t="n"/>
-      <c r="B20" s="83" t="n"/>
+      <c r="B20" s="84" t="n"/>
       <c r="C20" s="2" t="n"/>
       <c r="D20" s="2" t="n"/>
       <c r="E20" s="2" t="n"/>
@@ -3243,7 +3282,7 @@
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="F21" s="84" t="n"/>
+      <c r="F21" s="85" t="n"/>
       <c r="G21" s="56" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
@@ -3254,7 +3293,7 @@
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I21" s="85" t="inlineStr">
+      <c r="I21" s="86" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
@@ -3272,11 +3311,11 @@
       <c r="T21" s="2" t="n"/>
     </row>
     <row r="22" ht="27" customHeight="1">
-      <c r="A22" s="86" t="n"/>
-      <c r="B22" s="86" t="n"/>
-      <c r="C22" s="86" t="n"/>
-      <c r="D22" s="86" t="n"/>
-      <c r="E22" s="87" t="inlineStr">
+      <c r="A22" s="87" t="n"/>
+      <c r="B22" s="87" t="n"/>
+      <c r="C22" s="87" t="n"/>
+      <c r="D22" s="87" t="n"/>
+      <c r="E22" s="88" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
@@ -3286,9 +3325,9 @@
           <t>SF</t>
         </is>
       </c>
-      <c r="G22" s="86" t="n"/>
-      <c r="H22" s="86" t="n"/>
-      <c r="I22" s="86" t="n"/>
+      <c r="G22" s="87" t="n"/>
+      <c r="H22" s="87" t="n"/>
+      <c r="I22" s="87" t="n"/>
     </row>
     <row r="23" ht="27" customHeight="1">
       <c r="A23" s="58" t="inlineStr">
@@ -3307,7 +3346,7 @@
         </is>
       </c>
       <c r="D23" s="58" t="n"/>
-      <c r="E23" s="88" t="n">
+      <c r="E23" s="89" t="n">
         <v>122</v>
       </c>
       <c r="F23" s="59" t="n">
@@ -3319,7 +3358,7 @@
       <c r="H23" s="59" t="n">
         <v>512.1048</v>
       </c>
-      <c r="I23" s="89" t="n">
+      <c r="I23" s="90" t="n">
         <v>1.8312</v>
       </c>
     </row>
@@ -3340,7 +3379,7 @@
         </is>
       </c>
       <c r="D24" s="58" t="n"/>
-      <c r="E24" s="88" t="n">
+      <c r="E24" s="89" t="n">
         <v>2</v>
       </c>
       <c r="F24" s="59" t="n">
@@ -3352,7 +3391,7 @@
       <c r="H24" s="59" t="n">
         <v>8.395200000000001</v>
       </c>
-      <c r="I24" s="89" t="n">
+      <c r="I24" s="90" t="n">
         <v>0.03</v>
       </c>
     </row>
@@ -3373,7 +3412,7 @@
         </is>
       </c>
       <c r="D25" s="58" t="n"/>
-      <c r="E25" s="88" t="n">
+      <c r="E25" s="89" t="n">
         <v>190</v>
       </c>
       <c r="F25" s="59" t="n">
@@ -3385,7 +3424,7 @@
       <c r="H25" s="59" t="n">
         <v>802</v>
       </c>
-      <c r="I25" s="89" t="n">
+      <c r="I25" s="90" t="n">
         <v>2.4552</v>
       </c>
     </row>
@@ -3406,7 +3445,7 @@
         </is>
       </c>
       <c r="D26" s="58" t="n"/>
-      <c r="E26" s="88" t="n">
+      <c r="E26" s="89" t="n">
         <v>208</v>
       </c>
       <c r="F26" s="59" t="n">
@@ -3418,7 +3457,7 @@
       <c r="H26" s="59" t="n">
         <v>885.9439</v>
       </c>
-      <c r="I26" s="89" t="n">
+      <c r="I26" s="90" t="n">
         <v>2.6943</v>
       </c>
     </row>
@@ -3434,7 +3473,7 @@
         </is>
       </c>
       <c r="D27" s="58" t="n"/>
-      <c r="E27" s="88" t="n">
+      <c r="E27" s="89" t="n">
         <v>6</v>
       </c>
       <c r="F27" s="59" t="n">
@@ -3446,7 +3485,7 @@
       <c r="H27" s="59" t="n">
         <v>25.5561</v>
       </c>
-      <c r="I27" s="89" t="n">
+      <c r="I27" s="90" t="n">
         <v>0.07770000000000001</v>
       </c>
     </row>
@@ -3460,7 +3499,7 @@
         </is>
       </c>
       <c r="D28" s="58" t="n"/>
-      <c r="E28" s="88" t="n">
+      <c r="E28" s="89" t="n">
         <v>154</v>
       </c>
       <c r="F28" s="59" t="n">
@@ -3472,7 +3511,7 @@
       <c r="H28" s="59" t="n">
         <v>658.0814</v>
       </c>
-      <c r="I28" s="89" t="n">
+      <c r="I28" s="90" t="n">
         <v>2.0564</v>
       </c>
     </row>
@@ -3486,7 +3525,7 @@
         </is>
       </c>
       <c r="D29" s="58" t="n"/>
-      <c r="E29" s="88" t="n">
+      <c r="E29" s="89" t="n">
         <v>18</v>
       </c>
       <c r="F29" s="59" t="n">
@@ -3498,7 +3537,7 @@
       <c r="H29" s="59" t="n">
         <v>76.9186</v>
       </c>
-      <c r="I29" s="89" t="n">
+      <c r="I29" s="90" t="n">
         <v>0.2404</v>
       </c>
     </row>
@@ -3512,7 +3551,7 @@
         </is>
       </c>
       <c r="D30" s="58" t="n"/>
-      <c r="E30" s="88" t="n">
+      <c r="E30" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F30" s="59" t="n">
@@ -3524,7 +3563,7 @@
       <c r="H30" s="59" t="n">
         <v>859.5</v>
       </c>
-      <c r="I30" s="89" t="n">
+      <c r="I30" s="90" t="n">
         <v>2.376</v>
       </c>
     </row>
@@ -3538,7 +3577,7 @@
         </is>
       </c>
       <c r="D31" s="58" t="n"/>
-      <c r="E31" s="88" t="n">
+      <c r="E31" s="89" t="n">
         <v>200</v>
       </c>
       <c r="F31" s="59" t="n">
@@ -3550,7 +3589,7 @@
       <c r="H31" s="59" t="n">
         <v>780.1762</v>
       </c>
-      <c r="I31" s="89" t="n">
+      <c r="I31" s="90" t="n">
         <v>2.2678</v>
       </c>
     </row>
@@ -3564,7 +3603,7 @@
         </is>
       </c>
       <c r="D32" s="58" t="n"/>
-      <c r="E32" s="88" t="n">
+      <c r="E32" s="89" t="n">
         <v>27</v>
       </c>
       <c r="F32" s="59" t="n">
@@ -3576,7 +3615,7 @@
       <c r="H32" s="59" t="n">
         <v>105.3238</v>
       </c>
-      <c r="I32" s="89" t="n">
+      <c r="I32" s="90" t="n">
         <v>0.3062</v>
       </c>
     </row>
@@ -3590,7 +3629,7 @@
         </is>
       </c>
       <c r="D33" s="58" t="n"/>
-      <c r="E33" s="88" t="n">
+      <c r="E33" s="89" t="n">
         <v>169</v>
       </c>
       <c r="F33" s="59" t="n">
@@ -3602,7 +3641,7 @@
       <c r="H33" s="59" t="n">
         <v>736.84</v>
       </c>
-      <c r="I33" s="89" t="n">
+      <c r="I33" s="90" t="n">
         <v>2.2181</v>
       </c>
     </row>
@@ -3616,7 +3655,7 @@
         </is>
       </c>
       <c r="D34" s="58" t="n"/>
-      <c r="E34" s="88" t="n">
+      <c r="E34" s="89" t="n">
         <v>6</v>
       </c>
       <c r="F34" s="59" t="n">
@@ -3628,7 +3667,7 @@
       <c r="H34" s="59" t="n">
         <v>26.16</v>
       </c>
-      <c r="I34" s="89" t="n">
+      <c r="I34" s="90" t="n">
         <v>0.07870000000000001</v>
       </c>
     </row>
@@ -3642,7 +3681,7 @@
         </is>
       </c>
       <c r="D35" s="58" t="n"/>
-      <c r="E35" s="88" t="n">
+      <c r="E35" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F35" s="59" t="n">
@@ -3654,7 +3693,7 @@
       <c r="H35" s="59" t="n">
         <v>859.5</v>
       </c>
-      <c r="I35" s="89" t="n">
+      <c r="I35" s="90" t="n">
         <v>2.376</v>
       </c>
     </row>
@@ -3668,7 +3707,7 @@
         </is>
       </c>
       <c r="D36" s="58" t="n"/>
-      <c r="E36" s="88" t="n">
+      <c r="E36" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F36" s="59" t="n">
@@ -3680,7 +3719,7 @@
       <c r="H36" s="59" t="n">
         <v>875.5</v>
       </c>
-      <c r="I36" s="89" t="n">
+      <c r="I36" s="90" t="n">
         <v>2.6136</v>
       </c>
     </row>
@@ -3694,7 +3733,7 @@
         </is>
       </c>
       <c r="D37" s="58" t="n"/>
-      <c r="E37" s="88" t="n">
+      <c r="E37" s="89" t="n">
         <v>215</v>
       </c>
       <c r="F37" s="59" t="n">
@@ -3706,7 +3745,7 @@
       <c r="H37" s="59" t="n">
         <v>946.5</v>
       </c>
-      <c r="I37" s="89" t="n">
+      <c r="I37" s="90" t="n">
         <v>2.97</v>
       </c>
     </row>
@@ -3720,7 +3759,7 @@
         </is>
       </c>
       <c r="D38" s="58" t="n"/>
-      <c r="E38" s="88" t="n">
+      <c r="E38" s="89" t="n">
         <v>215</v>
       </c>
       <c r="F38" s="59" t="n">
@@ -3732,7 +3771,7 @@
       <c r="H38" s="59" t="n">
         <v>963</v>
       </c>
-      <c r="I38" s="89" t="n">
+      <c r="I38" s="90" t="n">
         <v>2.6136</v>
       </c>
     </row>
@@ -3746,7 +3785,7 @@
         </is>
       </c>
       <c r="D39" s="58" t="n"/>
-      <c r="E39" s="88" t="n">
+      <c r="E39" s="89" t="n">
         <v>192</v>
       </c>
       <c r="F39" s="59" t="n">
@@ -3758,7 +3797,7 @@
       <c r="H39" s="59" t="n">
         <v>836.9709</v>
       </c>
-      <c r="I39" s="89" t="n">
+      <c r="I39" s="90" t="n">
         <v>2.4729</v>
       </c>
     </row>
@@ -3772,7 +3811,7 @@
         </is>
       </c>
       <c r="D40" s="58" t="n"/>
-      <c r="E40" s="88" t="n">
+      <c r="E40" s="89" t="n">
         <v>14</v>
       </c>
       <c r="F40" s="59" t="n">
@@ -3784,7 +3823,7 @@
       <c r="H40" s="59" t="n">
         <v>61.0291</v>
       </c>
-      <c r="I40" s="89" t="n">
+      <c r="I40" s="90" t="n">
         <v>0.1803</v>
       </c>
     </row>
@@ -3798,7 +3837,7 @@
         </is>
       </c>
       <c r="D41" s="58" t="n"/>
-      <c r="E41" s="88" t="n">
+      <c r="E41" s="89" t="n">
         <v>97</v>
       </c>
       <c r="F41" s="59" t="n">
@@ -3810,7 +3849,7 @@
       <c r="H41" s="59" t="n">
         <v>453</v>
       </c>
-      <c r="I41" s="89" t="n">
+      <c r="I41" s="90" t="n">
         <v>1.782</v>
       </c>
     </row>
@@ -3824,7 +3863,7 @@
         </is>
       </c>
       <c r="D42" s="58" t="n"/>
-      <c r="E42" s="88" t="n">
+      <c r="E42" s="89" t="n">
         <v>97</v>
       </c>
       <c r="F42" s="59" t="n">
@@ -3836,7 +3875,7 @@
       <c r="H42" s="59" t="n">
         <v>452</v>
       </c>
-      <c r="I42" s="89" t="n">
+      <c r="I42" s="90" t="n">
         <v>1.8216</v>
       </c>
     </row>
@@ -3850,7 +3889,7 @@
         </is>
       </c>
       <c r="D43" s="58" t="n"/>
-      <c r="E43" s="88" t="n">
+      <c r="E43" s="89" t="n">
         <v>184</v>
       </c>
       <c r="F43" s="59" t="n">
@@ -3862,7 +3901,7 @@
       <c r="H43" s="59" t="n">
         <v>817.3474</v>
       </c>
-      <c r="I43" s="89" t="n">
+      <c r="I43" s="90" t="n">
         <v>2.6461</v>
       </c>
     </row>
@@ -3876,7 +3915,7 @@
         </is>
       </c>
       <c r="D44" s="58" t="n"/>
-      <c r="E44" s="88" t="n">
+      <c r="E44" s="89" t="n">
         <v>6</v>
       </c>
       <c r="F44" s="59" t="n">
@@ -3888,7 +3927,7 @@
       <c r="H44" s="59" t="n">
         <v>26.6526</v>
       </c>
-      <c r="I44" s="89" t="n">
+      <c r="I44" s="90" t="n">
         <v>0.0863</v>
       </c>
     </row>
@@ -3902,7 +3941,7 @@
         </is>
       </c>
       <c r="D45" s="58" t="n"/>
-      <c r="E45" s="88" t="n">
+      <c r="E45" s="89" t="n">
         <v>185</v>
       </c>
       <c r="F45" s="59" t="n">
@@ -3914,7 +3953,7 @@
       <c r="H45" s="59" t="n">
         <v>830.0658</v>
       </c>
-      <c r="I45" s="89" t="n">
+      <c r="I45" s="90" t="n">
         <v>2.5063</v>
       </c>
     </row>
@@ -3928,7 +3967,7 @@
         </is>
       </c>
       <c r="D46" s="58" t="n"/>
-      <c r="E46" s="88" t="n">
+      <c r="E46" s="89" t="n">
         <v>5</v>
       </c>
       <c r="F46" s="59" t="n">
@@ -3940,7 +3979,7 @@
       <c r="H46" s="59" t="n">
         <v>22.4342</v>
       </c>
-      <c r="I46" s="89" t="n">
+      <c r="I46" s="90" t="n">
         <v>0.0677</v>
       </c>
     </row>
@@ -3954,7 +3993,7 @@
         </is>
       </c>
       <c r="D47" s="58" t="n"/>
-      <c r="E47" s="88" t="n">
+      <c r="E47" s="89" t="n">
         <v>190</v>
       </c>
       <c r="F47" s="59" t="n">
@@ -3966,7 +4005,7 @@
       <c r="H47" s="59" t="n">
         <v>869</v>
       </c>
-      <c r="I47" s="89" t="n">
+      <c r="I47" s="90" t="n">
         <v>2.574</v>
       </c>
     </row>
@@ -3980,7 +4019,7 @@
         </is>
       </c>
       <c r="D48" s="58" t="n"/>
-      <c r="E48" s="88" t="n">
+      <c r="E48" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F48" s="59" t="n">
@@ -3992,7 +4031,7 @@
       <c r="H48" s="59" t="n">
         <v>866</v>
       </c>
-      <c r="I48" s="89" t="n">
+      <c r="I48" s="90" t="n">
         <v>2.574</v>
       </c>
     </row>
@@ -4006,7 +4045,7 @@
         </is>
       </c>
       <c r="D49" s="58" t="n"/>
-      <c r="E49" s="88" t="n">
+      <c r="E49" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F49" s="59" t="n">
@@ -4018,7 +4057,7 @@
       <c r="H49" s="59" t="n">
         <v>870.5</v>
       </c>
-      <c r="I49" s="89" t="n">
+      <c r="I49" s="90" t="n">
         <v>2.4948</v>
       </c>
     </row>
@@ -4032,7 +4071,7 @@
         </is>
       </c>
       <c r="D50" s="58" t="n"/>
-      <c r="E50" s="88" t="n">
+      <c r="E50" s="89" t="n">
         <v>89</v>
       </c>
       <c r="F50" s="59" t="n">
@@ -4044,7 +4083,7 @@
       <c r="H50" s="59" t="n">
         <v>415.0481</v>
       </c>
-      <c r="I50" s="89" t="n">
+      <c r="I50" s="90" t="n">
         <v>1.4572</v>
       </c>
     </row>
@@ -4058,7 +4097,7 @@
         </is>
       </c>
       <c r="D51" s="58" t="n"/>
-      <c r="E51" s="88" t="n">
+      <c r="E51" s="89" t="n">
         <v>8</v>
       </c>
       <c r="F51" s="59" t="n">
@@ -4070,7 +4109,7 @@
       <c r="H51" s="59" t="n">
         <v>37.3077</v>
       </c>
-      <c r="I51" s="89" t="n">
+      <c r="I51" s="90" t="n">
         <v>0.131</v>
       </c>
     </row>
@@ -4084,7 +4123,7 @@
         </is>
       </c>
       <c r="D52" s="58" t="n"/>
-      <c r="E52" s="88" t="n">
+      <c r="E52" s="89" t="n">
         <v>7</v>
       </c>
       <c r="F52" s="59" t="n">
@@ -4096,21 +4135,39 @@
       <c r="H52" s="59" t="n">
         <v>32.6442</v>
       </c>
-      <c r="I52" s="89" t="n">
+      <c r="I52" s="90" t="n">
         <v>0.1146</v>
       </c>
     </row>
-    <row r="53" ht="27" customHeight="1"/>
+    <row r="53" ht="27" customHeight="1">
+      <c r="A53" s="91" t="n"/>
+      <c r="B53" s="55" t="inlineStr">
+        <is>
+          <t>LEATHER (HS.CODE: 4107.12.00)</t>
+        </is>
+      </c>
+      <c r="C53" s="55" t="n"/>
+      <c r="D53" s="55" t="n"/>
+      <c r="E53" s="88" t="n"/>
+      <c r="F53" s="56" t="n"/>
+      <c r="G53" s="56" t="n"/>
+      <c r="H53" s="56" t="n"/>
+      <c r="I53" s="86" t="n"/>
+    </row>
     <row r="54" ht="27" customHeight="1">
-      <c r="A54" s="55" t="inlineStr">
+      <c r="A54" s="55" t="n"/>
+      <c r="B54" s="55" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="B54" s="84" t="n"/>
-      <c r="C54" s="55" t="n"/>
+      <c r="C54" s="55" t="inlineStr">
+        <is>
+          <t>20 PALLETS</t>
+        </is>
+      </c>
       <c r="D54" s="55" t="n"/>
-      <c r="E54" s="87">
+      <c r="E54" s="88">
         <f>SUM(E23:E52)</f>
         <v/>
       </c>
@@ -4126,7 +4183,7 @@
         <f>SUM(H23:H52)</f>
         <v/>
       </c>
-      <c r="I54" s="85">
+      <c r="I54" s="86">
         <f>SUM(I23:I52)</f>
         <v/>
       </c>
@@ -4157,7 +4214,7 @@
           <t>Quantity(SF)</t>
         </is>
       </c>
-      <c r="F56" s="84" t="n"/>
+      <c r="F56" s="85" t="n"/>
       <c r="G56" s="56" t="inlineStr">
         <is>
           <t>N.W (kgs)</t>
@@ -4168,18 +4225,18 @@
           <t>G.W (kgs)</t>
         </is>
       </c>
-      <c r="I56" s="85" t="inlineStr">
+      <c r="I56" s="86" t="inlineStr">
         <is>
           <t>CBM</t>
         </is>
       </c>
     </row>
     <row r="57" ht="27" customHeight="1">
-      <c r="A57" s="86" t="n"/>
-      <c r="B57" s="86" t="n"/>
-      <c r="C57" s="86" t="n"/>
-      <c r="D57" s="86" t="n"/>
-      <c r="E57" s="87" t="inlineStr">
+      <c r="A57" s="87" t="n"/>
+      <c r="B57" s="87" t="n"/>
+      <c r="C57" s="87" t="n"/>
+      <c r="D57" s="87" t="n"/>
+      <c r="E57" s="88" t="inlineStr">
         <is>
           <t>PCS</t>
         </is>
@@ -4189,9 +4246,9 @@
           <t>SF</t>
         </is>
       </c>
-      <c r="G57" s="86" t="n"/>
-      <c r="H57" s="86" t="n"/>
-      <c r="I57" s="86" t="n"/>
+      <c r="G57" s="87" t="n"/>
+      <c r="H57" s="87" t="n"/>
+      <c r="I57" s="87" t="n"/>
     </row>
     <row r="58" ht="27" customHeight="1">
       <c r="A58" s="58" t="inlineStr">
@@ -4208,7 +4265,7 @@
         </is>
       </c>
       <c r="D58" s="58" t="n"/>
-      <c r="E58" s="88" t="n">
+      <c r="E58" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F58" s="59" t="n">
@@ -4220,7 +4277,7 @@
       <c r="H58" s="59" t="n">
         <v>887.5</v>
       </c>
-      <c r="I58" s="89" t="n">
+      <c r="I58" s="90" t="n">
         <v>2.6532</v>
       </c>
     </row>
@@ -4239,7 +4296,7 @@
         </is>
       </c>
       <c r="D59" s="58" t="n"/>
-      <c r="E59" s="88" t="n">
+      <c r="E59" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F59" s="59" t="n">
@@ -4251,7 +4308,7 @@
       <c r="H59" s="59" t="n">
         <v>891</v>
       </c>
-      <c r="I59" s="89" t="n">
+      <c r="I59" s="90" t="n">
         <v>2.4948</v>
       </c>
     </row>
@@ -4270,7 +4327,7 @@
         </is>
       </c>
       <c r="D60" s="58" t="n"/>
-      <c r="E60" s="88" t="n">
+      <c r="E60" s="89" t="n">
         <v>207</v>
       </c>
       <c r="F60" s="59" t="n">
@@ -4282,7 +4339,7 @@
       <c r="H60" s="59" t="n">
         <v>926.3013999999999</v>
       </c>
-      <c r="I60" s="89" t="n">
+      <c r="I60" s="90" t="n">
         <v>2.8447</v>
       </c>
     </row>
@@ -4301,7 +4358,7 @@
         </is>
       </c>
       <c r="D61" s="58" t="n"/>
-      <c r="E61" s="88" t="n">
+      <c r="E61" s="89" t="n">
         <v>12</v>
       </c>
       <c r="F61" s="59" t="n">
@@ -4313,7 +4370,7 @@
       <c r="H61" s="59" t="n">
         <v>53.6986</v>
       </c>
-      <c r="I61" s="89" t="n">
+      <c r="I61" s="90" t="n">
         <v>0.1649</v>
       </c>
     </row>
@@ -4327,7 +4384,7 @@
         </is>
       </c>
       <c r="D62" s="58" t="n"/>
-      <c r="E62" s="88" t="n">
+      <c r="E62" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F62" s="59" t="n">
@@ -4339,7 +4396,7 @@
       <c r="H62" s="59" t="n">
         <v>885</v>
       </c>
-      <c r="I62" s="89" t="n">
+      <c r="I62" s="90" t="n">
         <v>2.6136</v>
       </c>
     </row>
@@ -4353,7 +4410,7 @@
         </is>
       </c>
       <c r="D63" s="58" t="n"/>
-      <c r="E63" s="88" t="n">
+      <c r="E63" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F63" s="59" t="n">
@@ -4365,7 +4422,7 @@
       <c r="H63" s="59" t="n">
         <v>908.5</v>
       </c>
-      <c r="I63" s="89" t="n">
+      <c r="I63" s="90" t="n">
         <v>2.6928</v>
       </c>
     </row>
@@ -4379,7 +4436,7 @@
         </is>
       </c>
       <c r="D64" s="58" t="n"/>
-      <c r="E64" s="88" t="n">
+      <c r="E64" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F64" s="59" t="n">
@@ -4391,7 +4448,7 @@
       <c r="H64" s="59" t="n">
         <v>894</v>
       </c>
-      <c r="I64" s="89" t="n">
+      <c r="I64" s="90" t="n">
         <v>2.6136</v>
       </c>
     </row>
@@ -4405,7 +4462,7 @@
         </is>
       </c>
       <c r="D65" s="58" t="n"/>
-      <c r="E65" s="88" t="n">
+      <c r="E65" s="89" t="n">
         <v>175</v>
       </c>
       <c r="F65" s="59" t="n">
@@ -4417,7 +4474,7 @@
       <c r="H65" s="59" t="n">
         <v>780.2461</v>
       </c>
-      <c r="I65" s="89" t="n">
+      <c r="I65" s="90" t="n">
         <v>2.3339</v>
       </c>
     </row>
@@ -4431,7 +4488,7 @@
         </is>
       </c>
       <c r="D66" s="58" t="n"/>
-      <c r="E66" s="88" t="n">
+      <c r="E66" s="89" t="n">
         <v>18</v>
       </c>
       <c r="F66" s="59" t="n">
@@ -4443,7 +4500,7 @@
       <c r="H66" s="59" t="n">
         <v>80.2539</v>
       </c>
-      <c r="I66" s="89" t="n">
+      <c r="I66" s="90" t="n">
         <v>0.2401</v>
       </c>
     </row>
@@ -4457,7 +4514,7 @@
         </is>
       </c>
       <c r="D67" s="58" t="n"/>
-      <c r="E67" s="88" t="n">
+      <c r="E67" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F67" s="59" t="n">
@@ -4469,7 +4526,7 @@
       <c r="H67" s="59" t="n">
         <v>885</v>
       </c>
-      <c r="I67" s="89" t="n">
+      <c r="I67" s="90" t="n">
         <v>2.574</v>
       </c>
     </row>
@@ -4483,7 +4540,7 @@
         </is>
       </c>
       <c r="D68" s="58" t="n"/>
-      <c r="E68" s="88" t="n">
+      <c r="E68" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F68" s="59" t="n">
@@ -4495,7 +4552,7 @@
       <c r="H68" s="59" t="n">
         <v>889.5</v>
       </c>
-      <c r="I68" s="89" t="n">
+      <c r="I68" s="90" t="n">
         <v>2.772</v>
       </c>
     </row>
@@ -4509,7 +4566,7 @@
         </is>
       </c>
       <c r="D69" s="58" t="n"/>
-      <c r="E69" s="88" t="n">
+      <c r="E69" s="89" t="n">
         <v>195</v>
       </c>
       <c r="F69" s="59" t="n">
@@ -4521,7 +4578,7 @@
       <c r="H69" s="59" t="n">
         <v>888</v>
       </c>
-      <c r="I69" s="89" t="n">
+      <c r="I69" s="90" t="n">
         <v>2.6136</v>
       </c>
     </row>
@@ -4537,7 +4594,7 @@
         </is>
       </c>
       <c r="D70" s="58" t="n"/>
-      <c r="E70" s="88" t="n">
+      <c r="E70" s="89" t="n">
         <v>106</v>
       </c>
       <c r="F70" s="59" t="n">
@@ -4549,7 +4606,7 @@
       <c r="H70" s="59" t="n">
         <v>424.9725</v>
       </c>
-      <c r="I70" s="89" t="n">
+      <c r="I70" s="90" t="n">
         <v>2.0795</v>
       </c>
     </row>
@@ -4565,7 +4622,7 @@
         </is>
       </c>
       <c r="D71" s="58" t="n"/>
-      <c r="E71" s="88" t="n">
+      <c r="E71" s="89" t="n">
         <v>3</v>
       </c>
       <c r="F71" s="59" t="n">
@@ -4577,21 +4634,39 @@
       <c r="H71" s="59" t="n">
         <v>12.0275</v>
       </c>
-      <c r="I71" s="89" t="n">
+      <c r="I71" s="90" t="n">
         <v>0.0589</v>
       </c>
     </row>
-    <row r="72" ht="27" customHeight="1"/>
+    <row r="72" ht="27" customHeight="1">
+      <c r="A72" s="91" t="n"/>
+      <c r="B72" s="55" t="inlineStr">
+        <is>
+          <t>LEATHER (HS.CODE: 4107.12.00)</t>
+        </is>
+      </c>
+      <c r="C72" s="55" t="n"/>
+      <c r="D72" s="55" t="n"/>
+      <c r="E72" s="88" t="n"/>
+      <c r="F72" s="56" t="n"/>
+      <c r="G72" s="56" t="n"/>
+      <c r="H72" s="56" t="n"/>
+      <c r="I72" s="86" t="n"/>
+    </row>
     <row r="73" ht="27" customHeight="1">
-      <c r="A73" s="55" t="inlineStr">
+      <c r="A73" s="55" t="n"/>
+      <c r="B73" s="55" t="inlineStr">
         <is>
           <t>TOTAL:</t>
         </is>
       </c>
-      <c r="B73" s="84" t="n"/>
-      <c r="C73" s="55" t="n"/>
+      <c r="C73" s="55" t="inlineStr">
+        <is>
+          <t>11 PALLETS</t>
+        </is>
+      </c>
       <c r="D73" s="55" t="n"/>
-      <c r="E73" s="87">
+      <c r="E73" s="88">
         <f>SUM(E58:E71)</f>
         <v/>
       </c>
@@ -4607,71 +4682,75 @@
         <f>SUM(H58:H71)</f>
         <v/>
       </c>
-      <c r="I73" s="85">
+      <c r="I73" s="86">
         <f>SUM(I58:I71)</f>
         <v/>
       </c>
     </row>
+    <row r="74" ht="27" customHeight="1">
+      <c r="A74" s="92" t="n"/>
+      <c r="B74" s="92" t="inlineStr">
+        <is>
+          <t>TOTAL OF:</t>
+        </is>
+      </c>
+      <c r="C74" s="92" t="inlineStr">
+        <is>
+          <t>31 PALLETS</t>
+        </is>
+      </c>
+      <c r="D74" s="92" t="n"/>
+      <c r="E74" s="93">
+        <f>SUM(E23:E52,E58:E71)</f>
+        <v/>
+      </c>
+      <c r="F74" s="94">
+        <f>SUM(F23:F52,F58:F71)</f>
+        <v/>
+      </c>
+      <c r="G74" s="94">
+        <f>SUM(G23:G52,G58:G71)</f>
+        <v/>
+      </c>
+      <c r="H74" s="94">
+        <f>SUM(H23:H52,H58:H71)</f>
+        <v/>
+      </c>
+      <c r="I74" s="95">
+        <f>SUM(I23:I52,I58:I71)</f>
+        <v/>
+      </c>
+    </row>
     <row r="75" ht="27" customHeight="1">
-      <c r="A75" s="55" t="inlineStr">
-        <is>
-          <t>TOTAL OF:</t>
-        </is>
-      </c>
-      <c r="B75" s="84" t="n"/>
-      <c r="C75" s="55" t="n"/>
-      <c r="D75" s="55" t="n"/>
-      <c r="E75" s="87">
-        <f>SUM(E23:E52,E58:E71)</f>
-        <v/>
-      </c>
-      <c r="F75" s="56">
-        <f>SUM(F23:F52,F58:F71)</f>
-        <v/>
-      </c>
-      <c r="G75" s="56">
-        <f>SUM(G23:G52,G58:G71)</f>
-        <v/>
-      </c>
-      <c r="H75" s="56">
-        <f>SUM(H23:H52,H58:H71)</f>
-        <v/>
-      </c>
-      <c r="I75" s="85">
-        <f>SUM(I23:I52,I58:I71)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="76" ht="27" customHeight="1">
-      <c r="A76" s="2" t="n"/>
-      <c r="B76" s="2" t="n"/>
-      <c r="C76" s="2" t="n"/>
-      <c r="D76" s="2" t="n"/>
-      <c r="E76" s="2" t="n"/>
-      <c r="F76" s="2" t="n"/>
-      <c r="G76" s="2" t="n"/>
-      <c r="H76" s="2" t="n"/>
-      <c r="I76" s="2" t="n"/>
-      <c r="J76" s="2" t="n"/>
-      <c r="K76" s="2" t="n"/>
-      <c r="L76" s="2" t="n"/>
-      <c r="M76" s="2" t="n"/>
-      <c r="N76" s="2" t="n"/>
-      <c r="O76" s="2" t="n"/>
-      <c r="P76" s="2" t="n"/>
-      <c r="Q76" s="2" t="n"/>
-      <c r="R76" s="2" t="n"/>
-      <c r="S76" s="2" t="n"/>
-      <c r="T76" s="2" t="n"/>
+      <c r="A75" s="2" t="n"/>
+      <c r="B75" s="2" t="n"/>
+      <c r="C75" s="2" t="n"/>
+      <c r="D75" s="2" t="n"/>
+      <c r="E75" s="2" t="n"/>
+      <c r="F75" s="2" t="n"/>
+      <c r="G75" s="2" t="n"/>
+      <c r="H75" s="2" t="n"/>
+      <c r="I75" s="2" t="n"/>
+      <c r="J75" s="2" t="n"/>
+      <c r="K75" s="2" t="n"/>
+      <c r="L75" s="2" t="n"/>
+      <c r="M75" s="2" t="n"/>
+      <c r="N75" s="2" t="n"/>
+      <c r="O75" s="2" t="n"/>
+      <c r="P75" s="2" t="n"/>
+      <c r="Q75" s="2" t="n"/>
+      <c r="R75" s="2" t="n"/>
+      <c r="S75" s="2" t="n"/>
+      <c r="T75" s="2" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A73:B73"/>
+  <mergeCells count="27">
+    <mergeCell ref="B74"/>
+    <mergeCell ref="B72:C72"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="H56:H57"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="H21:H22"/>
-    <mergeCell ref="A54:B54"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="I56:I57"/>
     <mergeCell ref="A5:I5"/>
@@ -4680,9 +4759,11 @@
     <mergeCell ref="D56:D57"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="I21:I22"/>
-    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="B54"/>
     <mergeCell ref="A4:I4"/>
+    <mergeCell ref="B53:C53"/>
     <mergeCell ref="A21:A22"/>
+    <mergeCell ref="B73"/>
     <mergeCell ref="G56:G57"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="B56:B57"/>

</xml_diff>